<commit_message>
Update Sig. upregulated and downregulated metabolites.xlsx
</commit_message>
<xml_diff>
--- a/LA of metabolome data/1st metabolome LA results/Sig. upregulated and downregulated metabolites.xlsx
+++ b/LA of metabolome data/1st metabolome LA results/Sig. upregulated and downregulated metabolites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabde\OneDrive\Documents\UM documents\BMS Year 3\Internship + Thesis\Sabrina_BMS_Bachelor-Internship\R analysis of metabolome data\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34420f5773a88cdb/Documents/UM documents/BMS Year 3/Internship ^M Thesis/Sabrina_BMS_Bachelor-Internship/LA of metabolome data/1st metabolome LA results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B5AE39-26F5-4E50-9F4F-D188239F5DD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{73B5AE39-26F5-4E50-9F4F-D188239F5DD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{85581760-4082-41BF-8288-A546E7211B6A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-130" yWindow="0" windowWidth="10510" windowHeight="560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="38">
   <si>
     <t>HMDB</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>9 upregulated and 19 downregulated</t>
+  </si>
+  <si>
+    <t>up/down regulated using cutoff of +/- 1</t>
   </si>
 </sst>
 </file>
@@ -528,17 +531,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="7"/>
-    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -561,8 +564,8 @@
       <c r="F1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>36</v>
+      <c r="G1" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -584,6 +587,9 @@
       <c r="F2" t="s">
         <v>34</v>
       </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -604,6 +610,9 @@
       <c r="F3" t="s">
         <v>34</v>
       </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -624,6 +633,9 @@
       <c r="F4" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="G4" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -644,6 +656,9 @@
       <c r="F5" t="s">
         <v>34</v>
       </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
@@ -664,6 +679,9 @@
       <c r="F6" t="s">
         <v>34</v>
       </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
@@ -684,6 +702,9 @@
       <c r="F7" t="s">
         <v>34</v>
       </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
@@ -704,6 +725,9 @@
       <c r="F8" t="s">
         <v>34</v>
       </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -724,6 +748,9 @@
       <c r="F9" t="s">
         <v>34</v>
       </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
@@ -744,6 +771,9 @@
       <c r="F10" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="G10" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
@@ -764,6 +794,9 @@
       <c r="F11" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="G11" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -784,6 +817,9 @@
       <c r="F12" t="s">
         <v>34</v>
       </c>
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
@@ -804,6 +840,9 @@
       <c r="F13" t="s">
         <v>34</v>
       </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
@@ -824,6 +863,9 @@
       <c r="F14" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="G14" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
@@ -844,6 +886,9 @@
       <c r="F15" t="s">
         <v>34</v>
       </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
@@ -864,8 +909,11 @@
       <c r="F16" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -884,8 +932,11 @@
       <c r="F17" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -904,8 +955,11 @@
       <c r="F18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
@@ -924,8 +978,11 @@
       <c r="F19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -944,8 +1001,11 @@
       <c r="F20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
@@ -964,8 +1024,11 @@
       <c r="F21" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -984,8 +1047,11 @@
       <c r="F22" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -1004,8 +1070,11 @@
       <c r="F23" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
@@ -1024,8 +1093,11 @@
       <c r="F24" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
@@ -1044,8 +1116,11 @@
       <c r="F25" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
@@ -1064,8 +1139,11 @@
       <c r="F26" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
@@ -1084,8 +1162,11 @@
       <c r="F27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
@@ -1104,8 +1185,11 @@
       <c r="F28" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
@@ -1124,8 +1208,17 @@
       <c r="F29" t="s">
         <v>34</v>
       </c>
+      <c r="G29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F30" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>